<commit_message>
added functionality to parse the uploaded file and append the rows to the table
</commit_message>
<xml_diff>
--- a/uploads/TestData1.xlsx
+++ b/uploads/TestData1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian.clements\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{299A810A-2605-4ED1-9386-AE1BD3729E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781C4466-B643-4057-B3D7-96F1FB05E40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5250" windowWidth="29040" windowHeight="15840" xr2:uid="{B049B3FB-6490-465B-A439-65494C952FFB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Bobby Cortez</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>ernie@landmcustoms.com</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700DCF7C-93B9-4AD7-996E-5D582FD8DDFA}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,33 +456,41 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{4A447599-C399-42B9-BFF2-ABCB80BB2B75}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{64818901-06BF-4EFC-B42B-0F4627E7514B}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{47FF3784-512A-4E1A-A42D-1EC9E816E901}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4A447599-C399-42B9-BFF2-ABCB80BB2B75}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{64818901-06BF-4EFC-B42B-0F4627E7514B}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{47FF3784-512A-4E1A-A42D-1EC9E816E901}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>